<commit_message>
Remove dataset_description.xlsx row 'Value n'.
</commit_message>
<xml_diff>
--- a/mapclientplugins/generatesdsstep/resources/dataset_description.xlsx
+++ b/mapclientplugins/generatesdsstep/resources/dataset_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsor001/Projects/musculoskeletal/mapclientplugins/sparc/mapclientplugins.generatesds/mapclientplugins/generatesdsstep/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B2ED60-D1FA-C849-BDC9-7296FC99897D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29F8AF4-9DA9-0348-907E-B6B7577D9F8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22140" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>Metadata element</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Value 3</t>
-  </si>
-  <si>
-    <t>Value n</t>
   </si>
   <si>
     <t>Metadata Version</t>
@@ -954,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1005"/>
+  <dimension ref="A1:F1005"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,10 +964,10 @@
     <col min="3" max="3" width="31.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="7.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -989,394 +986,374 @@
       <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="11"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>11</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="18"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>15</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C6" s="15" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>18</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="C7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="B8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="C8" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="B9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="C9" s="24" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>27</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="C11" s="15" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>31</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="C12" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="C13" s="15" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>37</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="C14" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="15" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+      <c r="B15" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="C15" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="15" t="s">
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="B16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="C16" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="15" t="s">
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
+      <c r="B17" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="C17" s="26" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>49</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="18"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="C19" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="15" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
-        <v>54</v>
       </c>
       <c r="B20" s="27" t="str">
         <f>HYPERLINK("https://orcid.org/","ORCiD ID. If you don't have an ORCiD, we suggest you sign up for one.")</f>
         <v>ORCiD ID. If you don't have an ORCiD, we suggest you sign up for one.</v>
       </c>
       <c r="C20" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+      <c r="B21" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="C21" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="15" t="s">
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
+      <c r="B22" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="C22" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="D22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="21" t="s">
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="16" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>64</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="18"/>
       <c r="D23" s="19"/>
       <c r="E23" s="28"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="C24" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="29" t="s">
+      <c r="E24" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="29" t="s">
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
+      <c r="B25" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="C25" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="D25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
+      <c r="B26" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="C26" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="30" t="s">
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
+      <c r="B27" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="C27" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="15" t="s">
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
-        <v>79</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="18"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>80</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>81</v>
       </c>
       <c r="C29" s="15">
         <v>1</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>82</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>83</v>
       </c>
       <c r="C30" s="15">
         <v>0</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update generation of SDS to version 3.0.2.
</commit_message>
<xml_diff>
--- a/mapclientplugins/generatesdsstep/resources/dataset_description.xlsx
+++ b/mapclientplugins/generatesdsstep/resources/dataset_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsor001/Projects/musculoskeletal/mapclientplugins/sparc/mapclientplugins.generatesds/mapclientplugins/generatesdsstep/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hsor001/Projects/musculoskeletal/plugins/sparc/mapclientplugins.generatesds/mapclientplugins/generatesdsstep/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29F8AF4-9DA9-0348-907E-B6B7577D9F8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB5ECAD-6A17-F844-8E3E-E2450863053D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="22140" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14760" yWindow="-21100" windowWidth="29400" windowHeight="17400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>TG</author>
+    <author>Tom Gillespie</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -56,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="116">
   <si>
     <t>Metadata element</t>
   </si>
@@ -76,21 +78,48 @@
     <t>Value 3</t>
   </si>
   <si>
-    <t>Metadata Version</t>
-  </si>
-  <si>
-    <t>2.1.0</t>
+    <t>Value 4</t>
+  </si>
+  <si>
+    <t>Metadata version</t>
+  </si>
+  <si>
+    <t>3.0.1</t>
+  </si>
+  <si>
+    <t>3.0.2</t>
   </si>
   <si>
     <t>Type</t>
   </si>
   <si>
-    <t>The type of this dataset, specifically whether it is experimental or computation. The only valid values are experimental or computational. If experimental subjects are required, if computational, subjects are not required. Set to experimental by default, if you are submitting a computational study be sure to change it.</t>
+    <t>The type of this dataset, specifically whether it is experimental, computation, or device. The only valid values are experimental, computational, or device. If experimental subjects are required, if computational, subjects are not required. Set to experimental by default, if you are submitting a computational study be sure to change it.</t>
   </si>
   <si>
     <t>experimental</t>
   </si>
   <si>
+    <t>Standards information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Data standard</t>
+  </si>
+  <si>
+    <t>The specific data standards that this dataset conforms to. Examples of current know values are SPARC, HEAL, HEAL-REJOIN, and HEAL-PRECISION. This list may include mechanical standards, human curation standards, etc. List additional standards as separate columns.</t>
+  </si>
+  <si>
+    <t>SPARC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Data standard version</t>
+  </si>
+  <si>
+    <t>The version of the data standard. This is not the same as Metadata Version above.</t>
+  </si>
+  <si>
+    <t>3.0.0</t>
+  </si>
+  <si>
     <t>Basic information</t>
   </si>
   <si>
@@ -106,7 +135,16 @@
     <t xml:space="preserve">    Subtitle</t>
   </si>
   <si>
-    <t>NOTE This field is not currently used when publishing a SPARC dataset. Brief description of the study and the data set. Equivalent to the abstract of a scientific paper. Include the rationale for the approach, the types of data collected, the techniques used, formats and number of files and an approximate size. The metadata associated with the published version of this dataset does not currently make use of this field.</t>
+    <t>Need more than a title? Why not a subtitle!</t>
+  </si>
+  <si>
+    <t>That I worked really hard on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Description</t>
+  </si>
+  <si>
+    <t>Brief description of the study and the data set. Equivalent to the abstract of a scientific paper. Include the rationale for the approach, the types of data collected, the techniques used, formats and number of files and an approximate size</t>
   </si>
   <si>
     <t>A really cool dataset that I collected to answer some question.</t>
@@ -115,16 +153,16 @@
     <t xml:space="preserve">    Keywords</t>
   </si>
   <si>
-    <t>A set of keywords to assist in search.</t>
-  </si>
-  <si>
-    <t>spinal cord, electrophysiology, RNA-seq, mouse</t>
+    <t>A set of keywords to assist in search. Please provide one keyword per column.</t>
+  </si>
+  <si>
+    <t>spinal cord injury</t>
   </si>
   <si>
     <t xml:space="preserve">    Funding</t>
   </si>
   <si>
-    <t>Funding sources</t>
+    <t>Funding sources listed as free text.</t>
   </si>
   <si>
     <t>OT2OD025349</t>
@@ -137,6 +175,39 @@
   </si>
   <si>
     <t>Thank you everyone!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    License</t>
+  </si>
+  <si>
+    <t>The SPDX license identifier for the license for this dataset.</t>
+  </si>
+  <si>
+    <t>CC-BY-4.0</t>
+  </si>
+  <si>
+    <t>Funding information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Funding consortium</t>
+  </si>
+  <si>
+    <t>The consortium that funded the creation of this dataset.  If there was more than one add additional columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Funding agency</t>
+  </si>
+  <si>
+    <t>The agency that funded the creation of this dataset. If there was more than one add additional columns</t>
+  </si>
+  <si>
+    <t>NIH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Award number</t>
+  </si>
+  <si>
+    <t>The award number issued by the funding agency. If there are multiple award numbers pair them with the issuing agency.</t>
   </si>
   <si>
     <t>Study information</t>
@@ -259,18 +330,23 @@
 Creator
 CoInvestigator
 CorrespondingAuthor
+ContactPerson
 DataCollector
 DataCurator
 DataManager
 Distributor
 Editor
+HostingInstitution
 Producer
 ProjectLeader
 ProjectManager
 ProjectMember
+RegistrationAgency
+RegistrationAuthority
 RelatedPerson
 Researcher
 ResearchGroup
+RightsHolder
 Sponsor
 Supervisor
 WorkPackageLeader
@@ -280,12 +356,6 @@
     <t>DataCollector</t>
   </si>
   <si>
-    <t>PrincipalInvestigator</t>
-  </si>
-  <si>
-    <t>CorrespondingAuthor</t>
-  </si>
-  <si>
     <t>Related protocol, paper, dataset, etc.</t>
   </si>
   <si>
@@ -295,10 +365,7 @@
     <t>A description of the referent of the related identifier.</t>
   </si>
   <si>
-    <t>Protocol for dataset</t>
-  </si>
-  <si>
-    <t>Paper for dataset</t>
+    <t>The protocol use to generate this dataset.</t>
   </si>
   <si>
     <t xml:space="preserve">    Relation type</t>
@@ -310,12 +377,14 @@
 HasProtocol
 IsSoftwareFor
 HasSoftware
+SharesEntitiesWithDataset
 The DataCite list is:
 IsCitedBy,
 Cites,
 IsSupplementTo,
 IsSupplementedBy,
-IsContinuedByContinues,
+IsContinuedBy,
+Continues,
 IsDescribedBy,
 Describes,
 HasMetadata,
@@ -349,9 +418,6 @@
     <t>HasProtocol</t>
   </si>
   <si>
-    <t>IsDescribedBy</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Identifier</t>
   </si>
   <si>
@@ -364,7 +430,26 @@
     <t xml:space="preserve">    Identifier type</t>
   </si>
   <si>
-    <t>The type of the identifier.</t>
+    <t>The type of the identifier. Values:
+ARK
+arXiv
+bibcode
+DOI
+EAN13
+EISSN
+Handle
+IGSN
+ISBN
+ISSN
+ISTC
+LISSN
+LSID
+PMID
+PURL
+UPC
+URL
+URN
+w3id</t>
   </si>
   <si>
     <t>DOI</t>
@@ -385,7 +470,46 @@
     <t>Number of unique samples in this dataset, should match samples metadata file. Set to zero if there are no samples. Only required for experimental datasets.</t>
   </si>
   <si>
-    <t>The protocol used to generate this dataset.</t>
+    <t xml:space="preserve">    Number of sites</t>
+  </si>
+  <si>
+    <t>Number of unique sites in this dataset, should match sites metadata file. Set to zero if there are no sites. Only required for experimental datasets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Number of performances</t>
+  </si>
+  <si>
+    <t>Number of unique performances in this dataset, should match performances metadata file. Set to zero if there are no performances. Only required for experimental datasets.</t>
+  </si>
+  <si>
+    <t>Data dictionary information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Data dictionary path</t>
+  </si>
+  <si>
+    <t>The relative path from the top level of the dataset to the file defining the data dictionary.</t>
+  </si>
+  <si>
+    <t>code/my-data-dictionary.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Data dictionary type</t>
+  </si>
+  <si>
+    <t>The type of the data dictionary. Examples are json-schema, linkml, redcap, other. If you do not know what type you have please put other.</t>
+  </si>
+  <si>
+    <t>json-schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Data dictionary description</t>
+  </si>
+  <si>
+    <t>A description of the data dictionary, any standards it conforms to, how it is expected to be used to validate files, etc.</t>
+  </si>
+  <si>
+    <t>All json files in this dataset are expected to conform to this schema.</t>
   </si>
 </sst>
 </file>
@@ -395,7 +519,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -403,21 +527,35 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -425,16 +563,36 @@
       <sz val="12"/>
       <color rgb="FF1155CC"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,8 +629,14 @@
         <bgColor rgb="FFFFFF99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -495,95 +659,151 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+  <cellXfs count="39">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -671,10 +891,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -712,234 +932,128 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
-                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
-                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
+          <a:tileRect/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
-                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -951,425 +1065,617 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1005"/>
+  <dimension ref="A1:G1020"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="56.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="B5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="15" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="B6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="C6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="15" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
+      <c r="B10" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="C10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="B11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="C11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="D11" s="19"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="B12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="C12" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="D12" s="22"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+      <c r="B13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="C13" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13" t="s">
+      <c r="B14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="C14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
+      <c r="B17" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="C17" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="26" t="s">
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
+      <c r="B18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13" t="s">
+      <c r="C18" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="22"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+      <c r="C20" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="27" t="str">
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="26"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="27" t="str">
         <f>HYPERLINK("https://orcid.org/","ORCiD ID. If you don't have an ORCiD, we suggest you sign up for one.")</f>
         <v>ORCiD ID. If you don't have an ORCiD, we suggest you sign up for one.</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="19"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="15" t="s">
+      <c r="C29" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" s="15">
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="11">
         <v>1</v>
       </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" s="15">
+      <c r="D38" s="1">
         <v>0</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="11">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="11">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+    </row>
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="11">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" s="37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B45" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" s="36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2327,9 +2633,24 @@
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C26" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C35" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>